<commit_message>
Python version to excel
</commit_message>
<xml_diff>
--- a/invoice-python/pur_inv.xlsx
+++ b/invoice-python/pur_inv.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
-  <si>
-    <t>No. Of Container</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Invoice</t>
   </si>
@@ -57,9 +54,6 @@
     <t>5x2.5</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>7x40'</t>
   </si>
   <si>
@@ -91,6 +85,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Container</t>
   </si>
 </sst>
 </file>
@@ -927,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -938,56 +935,53 @@
     <col min="1" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -1022,16 +1016,13 @@
       <c r="M2" s="3">
         <v>0</v>
       </c>
-      <c r="N2" s="3">
-        <v>42450</v>
-      </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="C3" s="3">
         <v>200</v>
@@ -1066,16 +1057,13 @@
       <c r="M3" s="3">
         <v>0</v>
       </c>
-      <c r="N3" s="3">
-        <v>42450</v>
-      </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3">
         <v>600</v>
@@ -1110,16 +1098,13 @@
       <c r="M4" s="3">
         <v>50</v>
       </c>
-      <c r="N4" s="3">
-        <v>43700</v>
-      </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:13">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
@@ -1154,16 +1139,13 @@
       <c r="M5" s="3">
         <v>0</v>
       </c>
-      <c r="N5" s="3">
-        <v>47700</v>
-      </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3">
         <v>600</v>
@@ -1198,16 +1180,13 @@
       <c r="M6" s="3">
         <v>50</v>
       </c>
-      <c r="N6" s="3">
-        <v>47200</v>
-      </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:13">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3">
         <v>25200</v>
@@ -1234,7 +1213,7 @@
         <v>50</v>
       </c>
       <c r="K7" s="3">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="L7" s="3">
         <v>600</v>
@@ -1242,16 +1221,13 @@
       <c r="M7" s="3">
         <v>0</v>
       </c>
-      <c r="N7" s="3">
-        <v>47700</v>
-      </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3">
         <v>25200</v>
@@ -1286,16 +1262,13 @@
       <c r="M8" s="3">
         <v>0</v>
       </c>
-      <c r="N8" s="3">
-        <v>47700</v>
-      </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3">
         <v>104000</v>
@@ -1330,13 +1303,10 @@
       <c r="M9" s="3">
         <v>0</v>
       </c>
-      <c r="N9" s="3">
-        <v>158600</v>
-      </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:13">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="3:3">

</xml_diff>